<commit_message>
eddy ni 1988-1989 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8889/individueel_eindstand_dworp_12_8889.xlsx
+++ b/_data/ni/ni8889/individueel_eindstand_dworp_12_8889.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20880" windowHeight="12840"/>
+    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="175">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Jaar 2</t>
   </si>
   <si>
-    <t>Geraardsbergen</t>
-  </si>
-  <si>
     <t>Courteyn Patrick</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>Dethier G</t>
-  </si>
-  <si>
-    <t>Westland</t>
   </si>
   <si>
     <t>Lapierre</t>
@@ -248,9 +242,6 @@
   </si>
   <si>
     <t>Deklerck Willy</t>
-  </si>
-  <si>
-    <t>Soignies</t>
   </si>
   <si>
     <t>Vanderose</t>
@@ -352,9 +343,6 @@
     <t>Meckelynck</t>
   </si>
   <si>
-    <t>CRE Charleroi</t>
-  </si>
-  <si>
     <t>Piacentini</t>
   </si>
   <si>
@@ -373,9 +361,6 @@
     <t>Leonard</t>
   </si>
   <si>
-    <t>Pantin</t>
-  </si>
-  <si>
     <t>Johannes</t>
   </si>
   <si>
@@ -386,9 +371,6 @@
   </si>
   <si>
     <t>Onrubia</t>
-  </si>
-  <si>
-    <t>Thibaut</t>
   </si>
   <si>
     <t>Herzfeld</t>
@@ -407,9 +389,6 @@
   </si>
   <si>
     <t>Van Meenen</t>
-  </si>
-  <si>
-    <t>Chess Club</t>
   </si>
   <si>
     <t>Polarski</t>
@@ -478,9 +457,6 @@
     <t>Cuvelier</t>
   </si>
   <si>
-    <t>Roque 2</t>
-  </si>
-  <si>
     <t>Janssens Guy</t>
   </si>
   <si>
@@ -497,9 +473,6 @@
   </si>
   <si>
     <t>Debouvere Pascal</t>
-  </si>
-  <si>
-    <t>Wavre</t>
   </si>
   <si>
     <t>Westland 1</t>
@@ -532,10 +505,52 @@
     <t>Roque 5</t>
   </si>
   <si>
+    <t>Westland 3 gaf 3 maal forfait, de uitslagen blijven behouden ter informatie maar het totaal van 3 punten moet eigenlijk nul of ff zijn.</t>
+  </si>
+  <si>
     <t>bron: maandblad SVB 15/11/1988; NIC ronde 1</t>
   </si>
   <si>
-    <t>Westland 3 gaf 3 maal forfait, de uitslagen blijven behouden ter informatie</t>
+    <t>formules in die zin aangepast door Pieter en dan gepubliceerd</t>
+  </si>
+  <si>
+    <t>Tot mijn groot ongenoegen merk ik dat zelfs de nationale tornooileider de namen van de ploegen onvolledig nummert:</t>
+  </si>
+  <si>
+    <t>in reeks 3B staat er Wavre maar in reeks 4E staat er Wavre 2. De facto noteer ik in reeks 3B Wavre 1</t>
+  </si>
+  <si>
+    <t>op dezelfde manier nu ook</t>
+  </si>
+  <si>
+    <t>in reeks 3B staat er Westland maar in reeks 4E staat er Westland 3. De facto noteer ik in reeks 3B Westland 1</t>
+  </si>
+  <si>
+    <t>Thibaut 1</t>
+  </si>
+  <si>
+    <t>in reeks 3B staat er Thibaut maar in reeks 4E staat er Thibaut 2. De facto noteer ik in reeks 3B Thibaut 1</t>
+  </si>
+  <si>
+    <t>idem Gera 2 in reeks  5H en Charleroi 2 in reeks 5N  en Soignies 2 in reeks 5N</t>
+  </si>
+  <si>
+    <t>CRE Charleroi 1</t>
+  </si>
+  <si>
+    <t>Geraardsbergen 1</t>
+  </si>
+  <si>
+    <t>Soignies 1</t>
+  </si>
+  <si>
+    <t>idem Pantin 2 in reeks  5L en Chess Club 2 in reeks 5L</t>
+  </si>
+  <si>
+    <t>Chess Club 1</t>
+  </si>
+  <si>
+    <t>Pantin 1</t>
   </si>
 </sst>
 </file>
@@ -1629,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1669,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1677,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1694,7 +1709,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="C11" s="68" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
@@ -1709,14 +1724,143 @@
       <c r="N11" s="68"/>
       <c r="O11" s="68"/>
     </row>
-    <row r="13" spans="1:15">
-      <c r="C13" s="69" t="s">
+    <row r="12" spans="1:15">
+      <c r="C12" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="C16" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="C17" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" s="69" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1776,7 +1920,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -1818,7 +1962,7 @@
         <v>31526</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="18">
         <v>1989</v>
@@ -1834,7 +1978,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -1846,7 +1990,7 @@
         <v>19313</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="18">
         <v>1913</v>
@@ -1862,7 +2006,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -1874,7 +2018,7 @@
         <v>96246</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" s="18">
         <v>1910</v>
@@ -1890,7 +2034,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -1902,7 +2046,7 @@
         <v>2372</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D8" s="18">
         <v>1845</v>
@@ -1918,7 +2062,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -1930,7 +2074,7 @@
         <v>43419</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" s="18">
         <v>1751</v>
@@ -1946,7 +2090,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -1958,7 +2102,7 @@
         <v>33910</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D10" s="18">
         <v>1612</v>
@@ -1974,7 +2118,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -2021,7 +2165,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2063,7 +2207,7 @@
         <v>76325</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="18">
         <v>1900</v>
@@ -2079,7 +2223,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -2091,7 +2235,7 @@
         <v>31348</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="18">
         <v>1894</v>
@@ -2107,7 +2251,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -2119,7 +2263,7 @@
         <v>76317</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="18">
         <v>1859</v>
@@ -2135,7 +2279,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -2147,7 +2291,7 @@
         <v>27715</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18">
         <v>1713</v>
@@ -2163,7 +2307,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -3691,9 +3835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3802,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>37</v>
@@ -3949,7 +4091,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C5" s="41">
         <v>2.5</v>
@@ -4096,7 +4238,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="C6" s="41">
         <v>2</v>
@@ -4243,7 +4385,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="C7" s="41">
         <v>2.5</v>
@@ -4390,7 +4532,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="C8" s="41">
         <v>3</v>
@@ -4537,7 +4679,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>39</v>
+        <v>170</v>
       </c>
       <c r="C9" s="41">
         <v>1.5</v>
@@ -4684,7 +4826,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
       <c r="C10" s="41">
         <v>0.5</v>
@@ -4978,7 +5120,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C12" s="41">
         <v>1.5</v>
@@ -5125,7 +5267,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C13" s="41">
         <v>2</v>
@@ -5620,7 +5762,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>37</v>
@@ -5655,15 +5797,15 @@
       <c r="M18" s="41"/>
       <c r="N18" s="41"/>
       <c r="O18" s="42">
-        <f t="shared" ref="O18:O26" si="16">SUM(C18:K18)</f>
+        <f>SUM(C18:K18)</f>
         <v>20</v>
       </c>
       <c r="P18" s="43">
-        <f>SUM(S18:Z18)*2</f>
-        <v>11</v>
+        <f>SUM(S18:AA18)*2</f>
+        <v>12</v>
       </c>
       <c r="Q18" s="43">
-        <f t="shared" ref="Q18:Q29" si="17">COUNT(C18:N18)</f>
+        <f t="shared" ref="Q18:Q29" si="16">COUNT(C18:N18)</f>
         <v>9</v>
       </c>
       <c r="R18" s="52"/>
@@ -5767,7 +5909,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="C19" s="41">
         <v>2</v>
@@ -5802,15 +5944,15 @@
       <c r="M19" s="41"/>
       <c r="N19" s="41"/>
       <c r="O19" s="42">
+        <f t="shared" ref="O19:O29" si="17">SUM(C19:K19)</f>
+        <v>19.5</v>
+      </c>
+      <c r="P19" s="43">
+        <f t="shared" ref="P19:P27" si="18">SUM(S19:AA19)*2</f>
+        <v>11</v>
+      </c>
+      <c r="Q19" s="43">
         <f t="shared" si="16"/>
-        <v>19.5</v>
-      </c>
-      <c r="P19" s="43">
-        <f t="shared" ref="P19:P26" si="18">SUM(S19:Z19)*2</f>
-        <v>9</v>
-      </c>
-      <c r="Q19" s="43">
-        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="R19" s="52"/>
@@ -5914,7 +6056,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" s="41">
         <v>1.5</v>
@@ -5947,15 +6089,15 @@
       <c r="M20" s="41"/>
       <c r="N20" s="41"/>
       <c r="O20" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
       <c r="P20" s="43">
         <f t="shared" si="18"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q20" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="R20" s="52"/>
@@ -6059,7 +6201,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C21" s="41">
         <v>1.5</v>
@@ -6094,15 +6236,15 @@
       <c r="M21" s="41"/>
       <c r="N21" s="41"/>
       <c r="O21" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
       <c r="P21" s="43">
         <f t="shared" si="18"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q21" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="R21" s="52"/>
@@ -6241,15 +6383,15 @@
       <c r="M22" s="41"/>
       <c r="N22" s="41"/>
       <c r="O22" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="P22" s="43">
         <f t="shared" si="18"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q22" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="R22" s="52"/>
@@ -6353,7 +6495,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="41">
         <v>3</v>
@@ -6386,15 +6528,15 @@
       <c r="M23" s="41"/>
       <c r="N23" s="41"/>
       <c r="O23" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15.5</v>
       </c>
       <c r="P23" s="43">
         <f t="shared" si="18"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q23" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="R23" s="52"/>
@@ -6498,7 +6640,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" s="41">
         <v>1</v>
@@ -6531,7 +6673,7 @@
       <c r="M24" s="41"/>
       <c r="N24" s="41"/>
       <c r="O24" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.5</v>
       </c>
       <c r="P24" s="43">
@@ -6539,7 +6681,7 @@
         <v>5</v>
       </c>
       <c r="Q24" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="R24" s="52"/>
@@ -6643,7 +6785,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C25" s="41">
         <v>0.5</v>
@@ -6678,15 +6820,15 @@
       <c r="M25" s="41"/>
       <c r="N25" s="41"/>
       <c r="O25" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="P25" s="43">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="R25" s="52"/>
@@ -6790,7 +6932,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C26" s="41">
         <v>2</v>
@@ -6825,7 +6967,7 @@
       <c r="M26" s="41"/>
       <c r="N26" s="41"/>
       <c r="O26" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12.5</v>
       </c>
       <c r="P26" s="43">
@@ -6833,7 +6975,7 @@
         <v>4</v>
       </c>
       <c r="Q26" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="R26" s="52"/>
@@ -6937,7 +7079,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C27" s="41">
         <v>0</v>
@@ -6946,7 +7088,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F27" s="41">
         <v>2</v>
@@ -6955,10 +7097,10 @@
         <v>0.5</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I27" s="41" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="J27" s="41">
         <v>0.5</v>
@@ -6978,7 +7120,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="R27" s="52"/>
@@ -7101,11 +7243,11 @@
         <v>0</v>
       </c>
       <c r="P28" s="43">
-        <f t="shared" ref="P28:P29" si="20">SUM(S28:AD28)*2</f>
+        <f t="shared" ref="P19:P29" si="20">SUM(S28:AD28)*2</f>
         <v>0</v>
       </c>
       <c r="Q28" s="43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R28" s="52"/>
@@ -7232,7 +7374,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R29" s="52"/>
@@ -13698,7 +13840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -13747,7 +13889,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>39</v>
+        <v>170</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -13789,7 +13931,7 @@
         <v>68128</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="18">
         <v>2100</v>
@@ -13803,7 +13945,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -13815,7 +13957,7 @@
         <v>2283</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="18">
         <v>2004</v>
@@ -13829,7 +13971,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -13841,7 +13983,7 @@
         <v>31526</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="18">
         <v>1989</v>
@@ -13855,7 +13997,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -13867,7 +14009,7 @@
         <v>76333</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="18">
         <v>1955</v>
@@ -13881,7 +14023,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -13893,7 +14035,7 @@
         <v>19313</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="18">
         <v>1913</v>
@@ -13909,7 +14051,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -13921,7 +14063,7 @@
         <v>96246</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="18">
         <v>1910</v>
@@ -13937,7 +14079,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -13984,7 +14126,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -14026,7 +14168,7 @@
         <v>76325</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="18">
         <v>1900</v>
@@ -14042,7 +14184,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -14054,7 +14196,7 @@
         <v>76317</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="18">
         <v>1859</v>
@@ -14070,7 +14212,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -14082,7 +14224,7 @@
         <v>353</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="18">
         <v>1851</v>
@@ -14098,7 +14240,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -14110,7 +14252,7 @@
         <v>27715</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18">
         <v>1713</v>
@@ -14126,7 +14268,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -14435,7 +14577,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14475,7 +14617,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -14523,7 +14665,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -14537,7 +14679,7 @@
         <v>68128</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J5" s="18">
         <v>2100</v>
@@ -14549,7 +14691,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -14563,7 +14705,7 @@
         <v>2283</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="18">
         <v>2004</v>
@@ -14575,7 +14717,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -14589,7 +14731,7 @@
         <v>31526</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J7" s="18">
         <v>1989</v>
@@ -14601,7 +14743,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -14615,7 +14757,7 @@
         <v>76333</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J8" s="18">
         <v>1955</v>
@@ -14627,7 +14769,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -14643,7 +14785,7 @@
         <v>19313</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J9" s="18">
         <v>1913</v>
@@ -14655,7 +14797,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -14671,7 +14813,7 @@
         <v>96246</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J10" s="18">
         <v>1910</v>
@@ -14712,7 +14854,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -14760,7 +14902,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -14776,7 +14918,7 @@
         <v>76325</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" s="18">
         <v>1900</v>
@@ -14788,7 +14930,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -14804,7 +14946,7 @@
         <v>31348</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" s="18">
         <v>1894</v>
@@ -14816,7 +14958,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -14832,7 +14974,7 @@
         <v>353</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" s="18">
         <v>1851</v>
@@ -14844,7 +14986,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -14860,7 +15002,7 @@
         <v>27715</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="18">
         <v>1713</v>
@@ -15171,7 +15313,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15219,7 +15361,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15261,7 +15403,7 @@
         <v>68128</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="18">
         <v>2100</v>
@@ -15275,7 +15417,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -15287,7 +15429,7 @@
         <v>2283</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="18">
         <v>2004</v>
@@ -15301,7 +15443,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -15313,7 +15455,7 @@
         <v>31526</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="18">
         <v>1989</v>
@@ -15327,7 +15469,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -15339,7 +15481,7 @@
         <v>76333</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="18">
         <v>1955</v>
@@ -15353,7 +15495,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -15365,7 +15507,7 @@
         <v>19313</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="18">
         <v>1913</v>
@@ -15381,7 +15523,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -15393,7 +15535,7 @@
         <v>96246</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="18">
         <v>1910</v>
@@ -15409,7 +15551,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -15456,7 +15598,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -15498,7 +15640,7 @@
         <v>76325</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="18">
         <v>1900</v>
@@ -15514,7 +15656,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -15526,7 +15668,7 @@
         <v>31348</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="18">
         <v>1894</v>
@@ -15542,7 +15684,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -15554,7 +15696,7 @@
         <v>353</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="18">
         <v>1851</v>
@@ -15570,7 +15712,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -15582,7 +15724,7 @@
         <v>27715</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18">
         <v>1713</v>
@@ -15598,7 +15740,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -15907,7 +16049,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:J10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15945,7 +16087,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="2"/>
       <c r="C3" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -15993,7 +16135,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -16007,7 +16149,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J5" s="18">
         <v>2004</v>
@@ -16019,7 +16161,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -16033,7 +16175,7 @@
         <v>31526</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J6" s="18">
         <v>1989</v>
@@ -16045,7 +16187,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -16059,7 +16201,7 @@
         <v>76333</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J7" s="18">
         <v>1955</v>
@@ -16071,7 +16213,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -16085,7 +16227,7 @@
         <v>19313</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J8" s="18">
         <v>1913</v>
@@ -16097,7 +16239,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -16113,7 +16255,7 @@
         <v>96246</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J9" s="18">
         <v>1910</v>
@@ -16125,7 +16267,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -16141,7 +16283,7 @@
         <v>43419</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="18">
         <v>1751</v>
@@ -16180,7 +16322,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16228,7 +16370,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -16244,7 +16386,7 @@
         <v>31348</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J15" s="18">
         <v>1894</v>
@@ -16256,7 +16398,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -16272,7 +16414,7 @@
         <v>76317</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J16" s="18">
         <v>1859</v>
@@ -16284,7 +16426,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -16300,7 +16442,7 @@
         <v>353</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" s="18">
         <v>1851</v>
@@ -16312,7 +16454,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -16328,7 +16470,7 @@
         <v>27715</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="18">
         <v>1713</v>
@@ -16687,7 +16829,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -16729,7 +16871,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="18">
         <v>2004</v>
@@ -16743,7 +16885,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -16755,7 +16897,7 @@
         <v>31526</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="18">
         <v>1989</v>
@@ -16769,7 +16911,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -16781,7 +16923,7 @@
         <v>76333</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="18">
         <v>1955</v>
@@ -16795,7 +16937,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -16807,7 +16949,7 @@
         <v>19313</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="18">
         <v>1913</v>
@@ -16821,7 +16963,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -16833,7 +16975,7 @@
         <v>96246</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="18">
         <v>1910</v>
@@ -16849,7 +16991,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -16861,7 +17003,7 @@
         <v>76317</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="18">
         <v>1859</v>
@@ -16877,7 +17019,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -16924,7 +17066,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -16966,7 +17108,7 @@
         <v>76325</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="18">
         <v>1900</v>
@@ -16982,7 +17124,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -16994,7 +17136,7 @@
         <v>31348</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="18">
         <v>1894</v>
@@ -17010,7 +17152,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -17022,7 +17164,7 @@
         <v>353</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="18">
         <v>1851</v>
@@ -17038,7 +17180,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -17050,7 +17192,7 @@
         <v>27715</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18">
         <v>1713</v>
@@ -17066,7 +17208,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -17375,7 +17517,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:J10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17413,7 +17555,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="2"/>
       <c r="C3" s="15" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -17461,7 +17603,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -17477,7 +17619,7 @@
         <v>68128</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J5" s="18">
         <v>2100</v>
@@ -17489,7 +17631,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -17505,7 +17647,7 @@
         <v>2283</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="18">
         <v>2004</v>
@@ -17517,7 +17659,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -17533,7 +17675,7 @@
         <v>31526</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J7" s="18">
         <v>1989</v>
@@ -17545,7 +17687,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -17561,7 +17703,7 @@
         <v>19313</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J8" s="18">
         <v>1913</v>
@@ -17573,7 +17715,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -17589,7 +17731,7 @@
         <v>96246</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J9" s="18">
         <v>1910</v>
@@ -17601,7 +17743,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="12">
@@ -17617,7 +17759,7 @@
         <v>43419</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="18">
         <v>1751</v>
@@ -17656,7 +17798,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="15" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17704,7 +17846,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -17720,7 +17862,7 @@
         <v>76325</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" s="18">
         <v>1900</v>
@@ -17732,7 +17874,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -17748,7 +17890,7 @@
         <v>76317</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J16" s="18">
         <v>1859</v>
@@ -17760,7 +17902,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -17776,7 +17918,7 @@
         <v>353</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" s="18">
         <v>1851</v>
@@ -17788,7 +17930,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -17804,7 +17946,7 @@
         <v>27715</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="18">
         <v>1713</v>
@@ -18115,7 +18257,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18163,7 +18305,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -18205,7 +18347,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="18">
         <v>2004</v>
@@ -18221,7 +18363,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -18233,7 +18375,7 @@
         <v>31526</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="18">
         <v>1989</v>
@@ -18249,7 +18391,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -18261,7 +18403,7 @@
         <v>76333</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="18">
         <v>1955</v>
@@ -18277,7 +18419,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -18289,7 +18431,7 @@
         <v>19313</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="18">
         <v>1913</v>
@@ -18305,7 +18447,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -18317,7 +18459,7 @@
         <v>96246</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="18">
         <v>1910</v>
@@ -18333,7 +18475,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J9" s="18"/>
     </row>
@@ -18345,7 +18487,7 @@
         <v>9270</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D10" s="18">
         <v>1693</v>
@@ -18361,7 +18503,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J10" s="18"/>
     </row>
@@ -18408,7 +18550,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18450,7 +18592,7 @@
         <v>31348</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D15" s="18">
         <v>1894</v>
@@ -18466,7 +18608,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -18478,7 +18620,7 @@
         <v>76317</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="18">
         <v>1859</v>
@@ -18494,7 +18636,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -18506,7 +18648,7 @@
         <v>353</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="18">
         <v>1851</v>
@@ -18522,7 +18664,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -18534,7 +18676,7 @@
         <v>27715</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18">
         <v>1713</v>
@@ -18550,7 +18692,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -18899,7 +19041,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -18947,7 +19089,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -18963,7 +19105,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J5" s="18">
         <v>2004</v>
@@ -18975,7 +19117,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -18991,7 +19133,7 @@
         <v>31526</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J6" s="18">
         <v>1989</v>
@@ -19003,7 +19145,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -19019,7 +19161,7 @@
         <v>76333</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J7" s="18">
         <v>1955</v>
@@ -19031,7 +19173,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -19047,7 +19189,7 @@
         <v>19313</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J8" s="18">
         <v>1913</v>
@@ -19059,7 +19201,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="10">
@@ -19075,7 +19217,7 @@
         <v>96246</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J9" s="18">
         <v>1910</v>
@@ -19087,7 +19229,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="10">
@@ -19103,7 +19245,7 @@
         <v>43419</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="18">
         <v>1751</v>
@@ -19144,7 +19286,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -19192,7 +19334,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -19208,7 +19350,7 @@
         <v>76325</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" s="18">
         <v>1900</v>
@@ -19220,7 +19362,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -19236,7 +19378,7 @@
         <v>31348</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" s="18">
         <v>1894</v>
@@ -19248,7 +19390,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -19264,7 +19406,7 @@
         <v>76317</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J17" s="18">
         <v>1859</v>
@@ -19276,7 +19418,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -19292,7 +19434,7 @@
         <v>27715</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="18">
         <v>1713</v>

</xml_diff>